<commit_message>
added data to stats by wards section
</commit_message>
<xml_diff>
--- a/HMIS passwords.xlsx
+++ b/HMIS passwords.xlsx
@@ -86,10 +86,10 @@
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -384,52 +384,52 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
     </row>
     <row r="2" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2" t="s">
+      <c r="D2" s="3"/>
+      <c r="E2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="2"/>
+      <c r="F2" s="3"/>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="2">
         <v>110105407</v>
       </c>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3" t="s">
+      <c r="D3" s="2"/>
+      <c r="E3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="3"/>
+      <c r="F3" s="2"/>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="2">
         <v>110105408</v>
       </c>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3" t="s">
+      <c r="D4" s="2"/>
+      <c r="E4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="3"/>
+      <c r="F4" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="7">

</xml_diff>

<commit_message>
fixed bug with overflowing nurse details section for admins
</commit_message>
<xml_diff>
--- a/HMIS passwords.xlsx
+++ b/HMIS passwords.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TABI TABOT M\Desktop\Ebot's files\Hospital-management-system-FET-final-year-project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDEC5B74-DB20-429F-8E51-EF4BD2DAA9DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8F47A29-C875-4DE6-BAB7-B2CF202E4D69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>HMIS passwards</t>
   </si>
@@ -46,6 +46,9 @@
   </si>
   <si>
     <t>Adm-94dbce87</t>
+  </si>
+  <si>
+    <t>For sis Manyi's laptop</t>
   </si>
 </sst>
 </file>
@@ -366,18 +369,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:F3"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="E3" sqref="E3:F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
+    <col min="1" max="1" width="27.6328125" customWidth="1"/>
     <col min="3" max="4" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -386,7 +390,7 @@
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
     </row>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
         <v>2</v>
       </c>
@@ -399,7 +403,10 @@
       </c>
       <c r="F2" s="1"/>
     </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
       <c r="B3" t="s">
         <v>4</v>
       </c>

</xml_diff>